<commit_message>
Allow setting LAS file data from external DataFrame
Also involved re-jigging the integral read() function workings. Now
everything works directly from the LASFile.data 2D ndarray
to unwrapped.ipynb
spreadsheet.ipynb
notebooks/issues/test_df_curve_addition_on_export.ipynb
LAS file.ipynb
</commit_message>
<xml_diff>
--- a/notebooks/example.xlsx
+++ b/notebooks/example.xlsx
@@ -256,7 +256,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -548,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+  <s:sheetPr xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+    <s:pageSetUpPr/>
+  </s:sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -907,10 +907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+  <s:sheetPr xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+    <s:pageSetUpPr/>
+  </s:sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>